<commit_message>
Project Tutorial 1 - Introduction to Decision Tables is saved. Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
+++ b/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
@@ -4169,8 +4169,8 @@
       <c r="E62" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F62" s="48">
-        <v>700</v>
+      <c r="F62" s="48" t="n">
+        <v>705.0</v>
       </c>
       <c r="G62" s="12"/>
     </row>

</xml_diff>